<commit_message>
Changes for coordinate offset testing
</commit_message>
<xml_diff>
--- a/data/g2-0.99/workbook.xlsx
+++ b/data/g2-0.99/workbook.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>g54</t>
   </si>
@@ -39,18 +39,6 @@
     <t>g59</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
     <t>x-mm</t>
   </si>
   <si>
@@ -67,17 +55,15 @@
   </si>
   <si>
     <t>z-in</t>
-  </si>
-  <si>
-    <t>L20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -122,8 +108,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -161,16 +159,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -188,6 +184,12 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -205,6 +207,12 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -534,543 +542,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:L19"/>
+  <dimension ref="A3:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="2" max="4" width="12" style="4" customWidth="1"/>
-    <col min="5" max="5" width="2.6640625" style="2" customWidth="1"/>
-    <col min="6" max="8" width="9.33203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="2.33203125" style="2" customWidth="1"/>
-    <col min="10" max="12" width="8.5" style="4" customWidth="1"/>
+    <col min="2" max="4" width="11.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="3.6640625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="10.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:12">
+    <row r="3" spans="1:8">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B5" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="F6" s="4">
-        <f>-B6</f>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <f>B5/25.4</f>
         <v>0</v>
       </c>
-      <c r="G6" s="4">
-        <f>-C6</f>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:H5" si="0">C5/25.4</f>
         <v>0</v>
       </c>
-      <c r="H6" s="4">
-        <f>-D6</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <f>F6/25.4</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <f>G6/25.4</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="4">
-        <f>H6/25.4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4">
-        <v>25.4</v>
-      </c>
-      <c r="C7" s="4">
-        <v>25.4</v>
-      </c>
-      <c r="D7" s="4">
-        <v>-12.7</v>
-      </c>
-      <c r="F7" s="4">
-        <f>-B7</f>
-        <v>-25.4</v>
-      </c>
-      <c r="G7" s="4">
-        <f>-C7</f>
-        <v>-25.4</v>
-      </c>
-      <c r="H7" s="4">
-        <f>-D7</f>
-        <v>12.7</v>
-      </c>
-      <c r="J7" s="4">
-        <f>F7/25.4</f>
-        <v>-1</v>
-      </c>
-      <c r="K7" s="4">
-        <f>G7/25.4</f>
-        <v>-1</v>
-      </c>
-      <c r="L7" s="4">
-        <f>H7/25.4</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="4">
-        <v>20</v>
-      </c>
-      <c r="C8" s="4">
-        <v>19</v>
-      </c>
-      <c r="D8" s="4">
-        <v>-10</v>
-      </c>
-      <c r="F8" s="4">
-        <f>-B8</f>
-        <v>-20</v>
-      </c>
-      <c r="G8" s="4">
-        <f>-C8</f>
-        <v>-19</v>
-      </c>
-      <c r="H8" s="4">
-        <f>-D8</f>
-        <v>10</v>
-      </c>
-      <c r="J8" s="4">
-        <f>F8/25.4</f>
-        <v>-0.78740157480314965</v>
-      </c>
-      <c r="K8" s="4">
-        <f>G8/25.4</f>
-        <v>-0.74803149606299213</v>
-      </c>
-      <c r="L8" s="4">
-        <f>H8/25.4</f>
-        <v>0.39370078740157483</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="4">
-        <v>14</v>
-      </c>
-      <c r="C9" s="4">
-        <v>14.1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>-8.6999999999999993</v>
-      </c>
-      <c r="F9" s="4">
-        <f>-B9</f>
-        <v>-14</v>
-      </c>
-      <c r="G9" s="4">
-        <f>-C9</f>
-        <v>-14.1</v>
-      </c>
-      <c r="H9" s="4">
-        <f>-D9</f>
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="J9" s="4">
-        <f>F9/25.4</f>
-        <v>-0.55118110236220474</v>
-      </c>
-      <c r="K9" s="4">
-        <f>G9/25.4</f>
-        <v>-0.55511811023622049</v>
-      </c>
-      <c r="L9" s="4">
-        <f>H9/25.4</f>
-        <v>0.34251968503937008</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="4">
-        <v>12</v>
-      </c>
-      <c r="C10" s="4">
-        <v>11</v>
-      </c>
-      <c r="D10" s="4">
-        <v>-6.3</v>
-      </c>
-      <c r="F10" s="4">
-        <f>-B10</f>
-        <v>-12</v>
-      </c>
-      <c r="G10" s="4">
-        <f>-C10</f>
-        <v>-11</v>
-      </c>
-      <c r="H10" s="4">
-        <f>-D10</f>
-        <v>6.3</v>
-      </c>
-      <c r="J10" s="4">
-        <f>F10/25.4</f>
-        <v>-0.47244094488188981</v>
-      </c>
-      <c r="K10" s="4">
-        <f>G10/25.4</f>
-        <v>-0.43307086614173229</v>
-      </c>
-      <c r="L10" s="4">
-        <f>H10/25.4</f>
-        <v>0.24803149606299213</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="4">
-        <v>11.5</v>
-      </c>
-      <c r="C11" s="4">
-        <v>6.6</v>
-      </c>
-      <c r="D11" s="4">
-        <v>-4.3</v>
-      </c>
-      <c r="F11" s="4">
-        <f>-B11</f>
-        <v>-11.5</v>
-      </c>
-      <c r="G11" s="4">
-        <f>-C11</f>
-        <v>-6.6</v>
-      </c>
-      <c r="H11" s="4">
-        <f>-D11</f>
-        <v>4.3</v>
-      </c>
-      <c r="J11" s="4">
-        <f>F11/25.4</f>
-        <v>-0.45275590551181105</v>
-      </c>
-      <c r="K11" s="4">
-        <f>G11/25.4</f>
-        <v>-0.25984251968503935</v>
-      </c>
-      <c r="L11" s="4">
-        <f>H11/25.4</f>
-        <v>0.16929133858267717</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="4">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="F14" s="4">
-        <f>B14</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" ref="G14:H14" si="0">C14</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J14" s="4">
-        <f>F14/25.4</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <f>G14/25.4</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="4">
-        <f>H14/25.4</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="A15" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B6" s="3">
         <v>25.4</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C6" s="3">
         <v>25.4</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D6" s="3">
         <v>-12.7</v>
       </c>
-      <c r="F15" s="4">
-        <f t="shared" ref="F15:F19" si="1">B15</f>
-        <v>25.4</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" ref="G15:G19" si="2">C15</f>
-        <v>25.4</v>
-      </c>
-      <c r="H15" s="4">
-        <f t="shared" ref="H15:H19" si="3">D15</f>
-        <v>-12.7</v>
-      </c>
-      <c r="J15" s="4">
-        <f t="shared" ref="J15:J19" si="4">F15/25.4</f>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <f t="shared" ref="F6:F10" si="1">B6/25.4</f>
         <v>1</v>
       </c>
-      <c r="K15" s="4">
-        <f t="shared" ref="K15:K19" si="5">G15/25.4</f>
+      <c r="G6" s="3">
+        <f t="shared" ref="G6:G10" si="2">C6/25.4</f>
         <v>1</v>
       </c>
-      <c r="L15" s="4">
-        <f t="shared" ref="L15:L19" si="6">H15/25.4</f>
+      <c r="H6" s="3">
+        <f t="shared" ref="H6:H10" si="3">D6/25.4</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B7" s="3">
         <v>20</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C7" s="3">
         <v>19</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D7" s="3">
         <v>-10</v>
       </c>
-      <c r="F16" s="4">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
         <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="G16" s="4">
+        <v>0.78740157480314965</v>
+      </c>
+      <c r="G7" s="3">
         <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="H16" s="4">
+        <v>0.74803149606299213</v>
+      </c>
+      <c r="H7" s="3">
         <f t="shared" si="3"/>
-        <v>-10</v>
-      </c>
-      <c r="J16" s="4">
-        <f t="shared" si="4"/>
-        <v>0.78740157480314965</v>
-      </c>
-      <c r="K16" s="4">
-        <f t="shared" si="5"/>
-        <v>0.74803149606299213</v>
-      </c>
-      <c r="L16" s="4">
-        <f t="shared" si="6"/>
         <v>-0.39370078740157483</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
-      <c r="A17" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B8" s="3">
         <v>14</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C8" s="3">
         <v>14.1</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D8" s="3">
         <v>-8.6999999999999993</v>
       </c>
-      <c r="F17" s="4">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="G17" s="4">
+        <v>0.55118110236220474</v>
+      </c>
+      <c r="G8" s="3">
         <f t="shared" si="2"/>
-        <v>14.1</v>
-      </c>
-      <c r="H17" s="4">
+        <v>0.55511811023622049</v>
+      </c>
+      <c r="H8" s="3">
         <f t="shared" si="3"/>
-        <v>-8.6999999999999993</v>
-      </c>
-      <c r="J17" s="4">
-        <f t="shared" si="4"/>
-        <v>0.55118110236220474</v>
-      </c>
-      <c r="K17" s="4">
-        <f t="shared" si="5"/>
-        <v>0.55511811023622049</v>
-      </c>
-      <c r="L17" s="4">
-        <f t="shared" si="6"/>
         <v>-0.34251968503937008</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B9" s="3">
         <v>12</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C9" s="3">
         <v>11</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D9" s="3">
         <v>-6.3</v>
       </c>
-      <c r="F18" s="4">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="G18" s="4">
+        <v>0.47244094488188981</v>
+      </c>
+      <c r="G9" s="3">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="H18" s="4">
+        <v>0.43307086614173229</v>
+      </c>
+      <c r="H9" s="3">
         <f t="shared" si="3"/>
-        <v>-6.3</v>
-      </c>
-      <c r="J18" s="4">
-        <f t="shared" si="4"/>
-        <v>0.47244094488188981</v>
-      </c>
-      <c r="K18" s="4">
-        <f t="shared" si="5"/>
-        <v>0.43307086614173229</v>
-      </c>
-      <c r="L18" s="4">
-        <f t="shared" si="6"/>
         <v>-0.24803149606299213</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
-      <c r="A19" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B10" s="3">
         <v>11.5</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C10" s="3">
         <v>6.6</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D10" s="3">
         <v>-4.3</v>
       </c>
-      <c r="F19" s="4">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
         <f t="shared" si="1"/>
-        <v>11.5</v>
-      </c>
-      <c r="G19" s="4">
+        <v>0.45275590551181105</v>
+      </c>
+      <c r="G10" s="3">
         <f t="shared" si="2"/>
-        <v>6.6</v>
-      </c>
-      <c r="H19" s="4">
+        <v>0.25984251968503935</v>
+      </c>
+      <c r="H10" s="3">
         <f t="shared" si="3"/>
-        <v>-4.3</v>
-      </c>
-      <c r="J19" s="4">
-        <f t="shared" si="4"/>
-        <v>0.45275590551181105</v>
-      </c>
-      <c r="K19" s="4">
-        <f t="shared" si="5"/>
-        <v>0.25984251968503935</v>
-      </c>
-      <c r="L19" s="4">
-        <f t="shared" si="6"/>
         <v>-0.16929133858267717</v>
       </c>
     </row>

</xml_diff>